<commit_message>
Fix trigger data references from breaking level editor
</commit_message>
<xml_diff>
--- a/Documentation/ClumsyBatIssuesList.xlsx
+++ b/Documentation/ClumsyBatIssuesList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
   <si>
     <t>Settings need to persist through sessions</t>
   </si>
@@ -86,15 +86,6 @@
     <t>bosshandler.cs</t>
   </si>
   <si>
-    <t>player.cs</t>
-  </si>
-  <si>
-    <t>DeactivateRush() being called too many times</t>
-  </si>
-  <si>
-    <t>Shield stats not implemented</t>
-  </si>
-  <si>
     <t>Pause game on completion (timer keeps going, can move player)</t>
   </si>
   <si>
@@ -264,6 +255,30 @@
   </si>
   <si>
     <t>Stat tracking (distance, durations etc) to be implemented</t>
+  </si>
+  <si>
+    <t>Finish levels</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Sound effects</t>
+  </si>
+  <si>
+    <t>Options menu remake</t>
+  </si>
+  <si>
+    <t>Mushroom spore angles not being reset on respawn</t>
+  </si>
+  <si>
+    <t>Bosses get stuck on ground when dashing</t>
+  </si>
+  <si>
+    <t>Spiders move to first block when hit</t>
+  </si>
+  <si>
+    <t>You win screen</t>
   </si>
 </sst>
 </file>
@@ -630,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -666,100 +681,182 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B35" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="4">
+        <v>43547</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B36" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C29" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
+      <c r="C36" s="4">
+        <v>43547</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B37" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="4">
+        <v>43547</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="4">
+        <v>43547</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B39" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="4">
+        <v>43547</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B40" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="4">
+        <v>43547</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B41" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="4">
+        <v>43547</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" s="4">
+        <v>43547</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="4">
+        <v>43547</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B44" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B32" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
-        <v>13</v>
+      <c r="C44" s="4">
+        <v>43547</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B45" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C45" s="4">
         <v>43547</v>
@@ -767,7 +864,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B46" s="3" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C46" s="4">
         <v>43547</v>
@@ -775,7 +872,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B47" s="3" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C47" s="4">
         <v>43547</v>
@@ -783,411 +880,371 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B48" s="3" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C48" s="4">
         <v>43547</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B49" s="3" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C49" s="4">
         <v>43547</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B50" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="4">
+        <v>43547</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B51" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51" s="6">
+        <v>43592</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B52" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="6">
+        <v>43592</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B53" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="6">
+        <v>43592</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B54" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" s="6">
+        <v>43592</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B55" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C55" s="6">
+        <v>43592</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B56" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C56" s="6">
+        <v>43593</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B57" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C57" s="6">
+        <v>43593</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B58" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58" s="6">
+        <v>43594</v>
+      </c>
+      <c r="E58" s="7"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B59" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C59" s="6">
+        <v>43594</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B60" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C60" s="6">
+        <v>43594</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B61" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C61" s="6">
+        <v>43594</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B62" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C62" s="6">
+        <v>43594</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B63" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C63" s="6">
+        <v>43594</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B64" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C64" s="6">
+        <v>43594</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B65" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C65" s="6">
+        <v>43600</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B66" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C66" s="6">
+        <v>43600</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B67" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C67" s="6">
+        <v>43600</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B68" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B69" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B70" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B71" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C71" s="6">
+        <v>43780</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B72" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C72" s="6">
+        <v>43780</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B73" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C73" s="6">
+        <v>43780</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B74" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C74" s="6">
+        <v>43780</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B75" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C75" s="6">
+        <v>43785</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B76" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C76" s="6">
+        <v>43785</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B77" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C77" s="6">
+        <v>43785</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B78" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C78" s="6">
+        <v>43785</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B79" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C79" s="6">
+        <v>43785</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B80" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C80" s="4">
+        <v>43786</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B81" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C81" s="4">
+        <v>43786</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B82" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C82" s="4">
+        <v>43786</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B83" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C83" s="4">
+        <v>43786</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B84" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C50" s="4">
-        <v>43547</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B51" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C51" s="4">
-        <v>43547</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B52" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C52" s="4">
-        <v>43547</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B53" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C53" s="4">
-        <v>43547</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B54" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C54" s="4">
-        <v>43547</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B55" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C55" s="4">
-        <v>43547</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B56" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" s="4">
-        <v>43547</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B57" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C57" s="4">
-        <v>43547</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B58" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C58" s="4">
-        <v>43547</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B59" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C59" s="4">
-        <v>43547</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B60" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C60" s="4">
-        <v>43547</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B61" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C61" s="6">
-        <v>43592</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B62" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C62" s="6">
-        <v>43592</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B63" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C63" s="6">
-        <v>43592</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B64" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C64" s="6">
-        <v>43592</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B65" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C65" s="6">
-        <v>43592</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B66" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C66" s="6">
-        <v>43593</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B67" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C67" s="6">
-        <v>43593</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B68" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C68" s="6">
-        <v>43594</v>
-      </c>
-      <c r="E68" s="7"/>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B69" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C69" s="6">
-        <v>43594</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B70" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C70" s="6">
-        <v>43594</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B71" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C71" s="6">
-        <v>43594</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B72" s="5" t="s">
+      <c r="C84" s="4">
+        <v>43792</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B85" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C85" s="4">
+        <v>43793</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B86" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C86" s="4">
+        <v>43793</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B87" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C87" s="4">
+        <v>43793</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B88" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C72" s="6">
-        <v>43594</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B73" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C73" s="6">
-        <v>43594</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B74" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C74" s="6">
-        <v>43594</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B75" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C75" s="6">
-        <v>43600</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B76" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C76" s="6">
-        <v>43600</v>
-      </c>
-    </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B77" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C77" s="6">
-        <v>43600</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B78" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B79" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B80" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B81" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C81" s="6">
-        <v>43780</v>
-      </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B82" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C82" s="6">
-        <v>43780</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B83" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C83" s="6">
-        <v>43780</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B84" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C84" s="6">
-        <v>43780</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B85" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C85" s="6">
-        <v>43785</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B86" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C86" s="6">
-        <v>43785</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B87" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C87" s="6">
-        <v>43785</v>
-      </c>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B88" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C88" s="6">
-        <v>43785</v>
+      <c r="C88" s="4">
+        <v>43793</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B89" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C89" s="6">
-        <v>43785</v>
+      <c r="B89" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C89" s="4">
+        <v>43794</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B90" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C90" s="4">
-        <v>43786</v>
+        <v>43794</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B91" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C91" s="4">
-        <v>43786</v>
+        <v>43795</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B92" s="3" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="C92" s="4">
-        <v>43786</v>
+        <v>43795</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B93" s="3" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="C93" s="4">
-        <v>43786</v>
-      </c>
-    </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B94" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C94" s="4">
-        <v>43792</v>
-      </c>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B95" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C95" s="4">
-        <v>43793</v>
-      </c>
-    </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B96" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C96" s="4">
-        <v>43793</v>
-      </c>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B97" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C97" s="4">
-        <v>43793</v>
-      </c>
-    </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B98" t="s">
-        <v>55</v>
-      </c>
-      <c r="C98" s="4">
-        <v>43793</v>
+        <v>43795</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Levels complete, audio starting to be added
Fix mushroom spore angle
Remove swinigng spiders - genuinely not worth the effort to fix bug given this is a demo game and no one will care
Level scores achievable
Removed the last few levels as part of the descoping process to complete the game - they don't add value
</commit_message>
<xml_diff>
--- a/Documentation/ClumsyBatIssuesList.xlsx
+++ b/Documentation/ClumsyBatIssuesList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
   <si>
     <t>Settings need to persist through sessions</t>
   </si>
@@ -279,6 +279,24 @@
   </si>
   <si>
     <t>You win screen</t>
+  </si>
+  <si>
+    <t>Not worth optimising, not the purpose of release</t>
+  </si>
+  <si>
+    <t>Not worth fixing, no one will notice or care</t>
+  </si>
+  <si>
+    <t>Not replicating through various replays. Not a game breaking bug either.</t>
+  </si>
+  <si>
+    <t>Swinging spiders drop after a set amount of time and shouldn’t ever drop…</t>
+  </si>
+  <si>
+    <t>Because this isn't a game that needs to be complete, we're descoping this</t>
+  </si>
+  <si>
+    <t>Unable to replicate</t>
   </si>
 </sst>
 </file>
@@ -645,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93:C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -681,11 +699,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>77</v>
-      </c>
-    </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>80</v>
@@ -700,6 +713,9 @@
       <c r="B6" t="s">
         <v>83</v>
       </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
@@ -716,67 +732,82 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+      <c r="C18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B25" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+      <c r="C24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
+    <row r="33" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B34" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="4">
+        <v>43547</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B35" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C35" s="4">
         <v>43547</v>
@@ -784,7 +815,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B36" s="3" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C36" s="4">
         <v>43547</v>
@@ -792,7 +823,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B37" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C37" s="4">
         <v>43547</v>
@@ -800,7 +831,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B38" s="3" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C38" s="4">
         <v>43547</v>
@@ -808,7 +839,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B39" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C39" s="4">
         <v>43547</v>
@@ -816,7 +847,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B40" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C40" s="4">
         <v>43547</v>
@@ -824,7 +855,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B41" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C41" s="4">
         <v>43547</v>
@@ -832,7 +863,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B42" s="3" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C42" s="4">
         <v>43547</v>
@@ -840,7 +871,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B43" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C43" s="4">
         <v>43547</v>
@@ -848,7 +879,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B44" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C44" s="4">
         <v>43547</v>
@@ -856,7 +887,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B45" s="3" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C45" s="4">
         <v>43547</v>
@@ -864,7 +895,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B46" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C46" s="4">
         <v>43547</v>
@@ -872,7 +903,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B47" s="3" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C47" s="4">
         <v>43547</v>
@@ -880,7 +911,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B48" s="3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C48" s="4">
         <v>43547</v>
@@ -888,23 +919,23 @@
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B49" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C49" s="4">
         <v>43547</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B50" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C50" s="4">
-        <v>43547</v>
+      <c r="B50" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="6">
+        <v>43592</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B51" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C51" s="6">
         <v>43592</v>
@@ -912,7 +943,7 @@
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B52" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C52" s="6">
         <v>43592</v>
@@ -920,7 +951,7 @@
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B53" s="5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C53" s="6">
         <v>43592</v>
@@ -928,7 +959,7 @@
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B54" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C54" s="6">
         <v>43592</v>
@@ -936,15 +967,15 @@
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B55" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C55" s="6">
-        <v>43592</v>
+        <v>43593</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B56" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C56" s="6">
         <v>43593</v>
@@ -952,24 +983,24 @@
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B57" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C57" s="6">
-        <v>43593</v>
-      </c>
+        <v>43594</v>
+      </c>
+      <c r="E57" s="7"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B58" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C58" s="6">
         <v>43594</v>
       </c>
-      <c r="E58" s="7"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B59" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C59" s="6">
         <v>43594</v>
@@ -977,7 +1008,7 @@
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B60" s="5" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C60" s="6">
         <v>43594</v>
@@ -985,7 +1016,7 @@
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B61" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C61" s="6">
         <v>43594</v>
@@ -993,7 +1024,7 @@
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B62" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C62" s="6">
         <v>43594</v>
@@ -1001,7 +1032,7 @@
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B63" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C63" s="6">
         <v>43594</v>
@@ -1009,15 +1040,15 @@
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B64" s="5" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C64" s="6">
-        <v>43594</v>
+        <v>43600</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B65" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C65" s="6">
         <v>43600</v>
@@ -1025,7 +1056,7 @@
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B66" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C66" s="6">
         <v>43600</v>
@@ -1033,15 +1064,15 @@
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B67" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C67" s="6">
-        <v>43600</v>
+        <v>58</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B68" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>66</v>
@@ -1049,31 +1080,31 @@
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B69" s="5" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B70" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>66</v>
+      <c r="B70" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C70" s="6">
+        <v>43780</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B71" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C71" s="6">
         <v>43780</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B72" s="6" t="s">
-        <v>59</v>
+      <c r="B72" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="C72" s="6">
         <v>43780</v>
@@ -1081,31 +1112,31 @@
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B73" s="5" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="C73" s="6">
         <v>43780</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B74" s="5" t="s">
-        <v>51</v>
+      <c r="B74" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="C74" s="6">
-        <v>43780</v>
+        <v>43785</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B75" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C75" s="6">
         <v>43785</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B76" s="6" t="s">
-        <v>62</v>
+      <c r="B76" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="C76" s="6">
         <v>43785</v>
@@ -1113,7 +1144,7 @@
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B77" s="5" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="C77" s="6">
         <v>43785</v>
@@ -1121,23 +1152,23 @@
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B78" s="5" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="C78" s="6">
         <v>43785</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B79" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C79" s="6">
-        <v>43785</v>
+      <c r="B79" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C79" s="4">
+        <v>43786</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B80" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C80" s="4">
         <v>43786</v>
@@ -1145,7 +1176,7 @@
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B81" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C81" s="4">
         <v>43786</v>
@@ -1153,7 +1184,7 @@
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B82" s="3" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C82" s="4">
         <v>43786</v>
@@ -1161,23 +1192,23 @@
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B83" s="3" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="C83" s="4">
-        <v>43786</v>
+        <v>43792</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B84" s="3" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="C84" s="4">
-        <v>43792</v>
+        <v>43793</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B85" s="3" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C85" s="4">
         <v>43793</v>
@@ -1185,7 +1216,7 @@
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B86" s="3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C86" s="4">
         <v>43793</v>
@@ -1193,7 +1224,7 @@
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B87" s="3" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="C87" s="4">
         <v>43793</v>
@@ -1201,15 +1232,15 @@
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B88" s="3" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="C88" s="4">
-        <v>43793</v>
+        <v>43794</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B89" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C89" s="4">
         <v>43794</v>
@@ -1217,15 +1248,15 @@
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B90" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C90" s="4">
-        <v>43794</v>
+        <v>43795</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B91" s="3" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="C91" s="4">
         <v>43795</v>
@@ -1233,7 +1264,7 @@
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B92" s="3" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C92" s="4">
         <v>43795</v>
@@ -1241,10 +1272,26 @@
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B93" s="3" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="C93" s="4">
-        <v>43795</v>
+        <v>43807</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B94" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C94" s="4">
+        <v>43807</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B95" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C95" s="4">
+        <v>43807</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding music and audio effects
</commit_message>
<xml_diff>
--- a/Documentation/ClumsyBatIssuesList.xlsx
+++ b/Documentation/ClumsyBatIssuesList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
   <si>
     <t>Settings need to persist through sessions</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>Unable to replicate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -663,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93:C95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -699,235 +702,249 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
         <v>83</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+    <row r="7" spans="1:5" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
         <v>88</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C12" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+    <row r="15" spans="1:5" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
         <v>61</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+    <row r="20" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B23" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
         <v>50</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C21" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
         <v>64</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C22" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
+    <row r="25" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
+    <row r="31" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="4">
+        <v>43547</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="4">
+        <v>43547</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" s="3" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C34" s="4">
         <v>43547</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" s="3" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C35" s="4">
         <v>43547</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" s="3" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C36" s="4">
         <v>43547</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37" s="3" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C37" s="4">
         <v>43547</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C38" s="4">
         <v>43547</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B39" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C39" s="4">
         <v>43547</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B40" s="3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C40" s="4">
         <v>43547</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C41" s="4">
         <v>43547</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B42" s="3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C42" s="4">
         <v>43547</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B43" s="3" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C43" s="4">
         <v>43547</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B44" s="3" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C44" s="4">
         <v>43547</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45" s="3" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C45" s="4">
         <v>43547</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C46" s="4">
         <v>43547</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B47" s="3" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C47" s="4">
         <v>43547</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B48" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" s="4">
-        <v>43547</v>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B48" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="6">
+        <v>43592</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B49" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C49" s="4">
-        <v>43547</v>
+      <c r="B49" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="6">
+        <v>43592</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B50" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C50" s="6">
         <v>43592</v>
@@ -935,7 +952,7 @@
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B51" s="5" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C51" s="6">
         <v>43592</v>
@@ -943,7 +960,7 @@
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B52" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C52" s="6">
         <v>43592</v>
@@ -951,48 +968,48 @@
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B53" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C53" s="6">
-        <v>43592</v>
+        <v>43593</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B54" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C54" s="6">
-        <v>43592</v>
+        <v>43593</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B55" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C55" s="6">
-        <v>43593</v>
-      </c>
+        <v>43594</v>
+      </c>
+      <c r="E55" s="7"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B56" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C56" s="6">
-        <v>43593</v>
+        <v>43594</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B57" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C57" s="6">
         <v>43594</v>
       </c>
-      <c r="E57" s="7"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B58" s="5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C58" s="6">
         <v>43594</v>
@@ -1000,7 +1017,7 @@
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B59" s="5" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C59" s="6">
         <v>43594</v>
@@ -1008,7 +1025,7 @@
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B60" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C60" s="6">
         <v>43594</v>
@@ -1016,7 +1033,7 @@
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B61" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C61" s="6">
         <v>43594</v>
@@ -1024,23 +1041,23 @@
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B62" s="5" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C62" s="6">
-        <v>43594</v>
+        <v>43600</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B63" s="5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C63" s="6">
-        <v>43594</v>
+        <v>43600</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B64" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C64" s="6">
         <v>43600</v>
@@ -1048,87 +1065,87 @@
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B65" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C65" s="6">
-        <v>43600</v>
+        <v>58</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B66" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C66" s="6">
-        <v>43600</v>
+        <v>55</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B67" s="5" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B68" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>66</v>
+      <c r="B68" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C68" s="6">
+        <v>43780</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B69" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>66</v>
+      <c r="B69" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C69" s="6">
+        <v>43780</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B70" s="6" t="s">
-        <v>57</v>
+      <c r="B70" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="C70" s="6">
         <v>43780</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B71" s="6" t="s">
-        <v>59</v>
+      <c r="B71" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="C71" s="6">
         <v>43780</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B72" s="5" t="s">
-        <v>36</v>
+      <c r="B72" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="C72" s="6">
-        <v>43780</v>
+        <v>43785</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B73" s="5" t="s">
-        <v>51</v>
+      <c r="B73" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C73" s="6">
-        <v>43780</v>
+        <v>43785</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B74" s="6" t="s">
-        <v>63</v>
+      <c r="B74" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="C74" s="6">
         <v>43785</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B75" s="6" t="s">
-        <v>62</v>
+      <c r="B75" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C75" s="6">
         <v>43785</v>
@@ -1136,31 +1153,31 @@
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B76" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C76" s="6">
         <v>43785</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B77" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C77" s="6">
-        <v>43785</v>
+      <c r="B77" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C77" s="4">
+        <v>43786</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B78" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C78" s="6">
-        <v>43785</v>
+      <c r="B78" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C78" s="4">
+        <v>43786</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B79" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C79" s="4">
         <v>43786</v>
@@ -1168,7 +1185,7 @@
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B80" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C80" s="4">
         <v>43786</v>
@@ -1176,31 +1193,31 @@
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B81" s="3" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="C81" s="4">
-        <v>43786</v>
+        <v>43792</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B82" s="3" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C82" s="4">
-        <v>43786</v>
+        <v>43793</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B83" s="3" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="C83" s="4">
-        <v>43792</v>
+        <v>43793</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B84" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C84" s="4">
         <v>43793</v>
@@ -1208,7 +1225,7 @@
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B85" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C85" s="4">
         <v>43793</v>
@@ -1216,39 +1233,39 @@
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B86" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C86" s="4">
-        <v>43793</v>
+        <v>43794</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B87" s="3" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="C87" s="4">
-        <v>43793</v>
+        <v>43794</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B88" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C88" s="4">
-        <v>43794</v>
+        <v>43795</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B89" s="3" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="C89" s="4">
-        <v>43794</v>
+        <v>43795</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B90" s="3" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="C90" s="4">
         <v>43795</v>
@@ -1256,42 +1273,31 @@
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B91" s="3" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="C91" s="4">
-        <v>43795</v>
+        <v>43807</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B92" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C92" s="4">
-        <v>43795</v>
+        <v>43807</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B93" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C93" s="4">
         <v>43807</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B94" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C94" s="4">
-        <v>43807</v>
-      </c>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B95" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C95" s="4">
-        <v>43807</v>
+      <c r="B94" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preparation for final release
Added credits to main menu. Fixed end screen
</commit_message>
<xml_diff>
--- a/Documentation/ClumsyBatIssuesList.xlsx
+++ b/Documentation/ClumsyBatIssuesList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
   <si>
     <t>Settings need to persist through sessions</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Tutorials</t>
   </si>
   <si>
-    <t>bosshandler.cs</t>
-  </si>
-  <si>
     <t>Pause game on completion (timer keeps going, can move player)</t>
   </si>
   <si>
@@ -287,19 +284,22 @@
     <t>Not worth fixing, no one will notice or care</t>
   </si>
   <si>
-    <t>Not replicating through various replays. Not a game breaking bug either.</t>
-  </si>
-  <si>
     <t>Swinging spiders drop after a set amount of time and shouldn’t ever drop…</t>
   </si>
   <si>
     <t>Because this isn't a game that needs to be complete, we're descoping this</t>
   </si>
   <si>
-    <t>Unable to replicate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
+    <t>not required, technically works</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Not a game breaking bug</t>
+  </si>
+  <si>
+    <t>people might figure it out…</t>
   </si>
 </sst>
 </file>
@@ -666,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -702,95 +702,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s">
-        <v>90</v>
-      </c>
-    </row>
     <row r="7" spans="1:5" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" t="s">
-        <v>89</v>
-      </c>
-    </row>
     <row r="15" spans="1:5" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" t="s">
-        <v>87</v>
-      </c>
-    </row>
     <row r="20" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" t="s">
-        <v>85</v>
-      </c>
-    </row>
     <row r="25" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
@@ -800,7 +729,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B32" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" s="4">
         <v>43547</v>
@@ -808,7 +737,7 @@
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C33" s="4">
         <v>43547</v>
@@ -832,7 +761,7 @@
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" s="4">
         <v>43547</v>
@@ -840,7 +769,7 @@
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C37" s="4">
         <v>43547</v>
@@ -848,7 +777,7 @@
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C38" s="4">
         <v>43547</v>
@@ -856,7 +785,7 @@
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B39" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C39" s="4">
         <v>43547</v>
@@ -872,7 +801,7 @@
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C41" s="4">
         <v>43547</v>
@@ -880,7 +809,7 @@
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B42" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C42" s="4">
         <v>43547</v>
@@ -904,7 +833,7 @@
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C45" s="4">
         <v>43547</v>
@@ -928,7 +857,7 @@
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B48" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C48" s="6">
         <v>43592</v>
@@ -936,7 +865,7 @@
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B49" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C49" s="6">
         <v>43592</v>
@@ -944,7 +873,7 @@
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B50" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C50" s="6">
         <v>43592</v>
@@ -952,7 +881,7 @@
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B51" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C51" s="6">
         <v>43592</v>
@@ -960,7 +889,7 @@
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B52" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C52" s="6">
         <v>43592</v>
@@ -968,7 +897,7 @@
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B53" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C53" s="6">
         <v>43593</v>
@@ -976,7 +905,7 @@
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B54" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C54" s="6">
         <v>43593</v>
@@ -984,7 +913,7 @@
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B55" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C55" s="6">
         <v>43594</v>
@@ -993,7 +922,7 @@
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B56" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C56" s="6">
         <v>43594</v>
@@ -1001,7 +930,7 @@
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B57" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C57" s="6">
         <v>43594</v>
@@ -1009,7 +938,7 @@
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B58" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C58" s="6">
         <v>43594</v>
@@ -1017,7 +946,7 @@
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B59" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C59" s="6">
         <v>43594</v>
@@ -1025,7 +954,7 @@
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B60" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C60" s="6">
         <v>43594</v>
@@ -1033,7 +962,7 @@
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B61" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C61" s="6">
         <v>43594</v>
@@ -1041,7 +970,7 @@
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B62" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C62" s="6">
         <v>43600</v>
@@ -1049,7 +978,7 @@
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B63" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C63" s="6">
         <v>43600</v>
@@ -1057,7 +986,7 @@
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B64" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C64" s="6">
         <v>43600</v>
@@ -1065,31 +994,31 @@
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B65" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B66" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B67" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B68" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C68" s="6">
         <v>43780</v>
@@ -1097,7 +1026,7 @@
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B69" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C69" s="6">
         <v>43780</v>
@@ -1105,7 +1034,7 @@
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B70" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C70" s="6">
         <v>43780</v>
@@ -1113,7 +1042,7 @@
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B71" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C71" s="6">
         <v>43780</v>
@@ -1121,7 +1050,7 @@
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B72" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C72" s="6">
         <v>43785</v>
@@ -1129,7 +1058,7 @@
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B73" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C73" s="6">
         <v>43785</v>
@@ -1137,7 +1066,7 @@
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B74" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C74" s="6">
         <v>43785</v>
@@ -1153,7 +1082,7 @@
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B76" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C76" s="6">
         <v>43785</v>
@@ -1161,7 +1090,7 @@
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B77" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C77" s="4">
         <v>43786</v>
@@ -1169,7 +1098,7 @@
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B78" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C78" s="4">
         <v>43786</v>
@@ -1177,7 +1106,7 @@
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B79" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C79" s="4">
         <v>43786</v>
@@ -1185,7 +1114,7 @@
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B80" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C80" s="4">
         <v>43786</v>
@@ -1193,7 +1122,7 @@
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B81" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C81" s="4">
         <v>43792</v>
@@ -1201,7 +1130,7 @@
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B82" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C82" s="4">
         <v>43793</v>
@@ -1209,7 +1138,7 @@
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B83" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C83" s="4">
         <v>43793</v>
@@ -1217,7 +1146,7 @@
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B84" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C84" s="4">
         <v>43793</v>
@@ -1225,7 +1154,7 @@
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B85" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C85" s="4">
         <v>43793</v>
@@ -1233,7 +1162,7 @@
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B86" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C86" s="4">
         <v>43794</v>
@@ -1241,7 +1170,7 @@
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B87" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C87" s="4">
         <v>43794</v>
@@ -1249,7 +1178,7 @@
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B88" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C88" s="4">
         <v>43795</v>
@@ -1257,7 +1186,7 @@
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B89" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C89" s="4">
         <v>43795</v>
@@ -1265,7 +1194,7 @@
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B90" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C90" s="4">
         <v>43795</v>
@@ -1273,7 +1202,7 @@
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B91" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C91" s="4">
         <v>43807</v>
@@ -1281,7 +1210,7 @@
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B92" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C92" s="4">
         <v>43807</v>
@@ -1289,15 +1218,98 @@
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B93" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C93" s="4">
         <v>43807</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B94" t="s">
+      <c r="B94" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B95" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B96" s="3" t="s">
         <v>82</v>
+      </c>
+      <c r="C96" s="4">
+        <v>43469</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B97" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C97" s="4">
+        <v>43469</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B98" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C98" s="4">
+        <v>43469</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B99" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B100" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B101" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B102" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B103" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B104" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>